<commit_message>
final changes to finance midterm
</commit_message>
<xml_diff>
--- a/midterm_accounting/EX1_Complete_formatted.xlsx
+++ b/midterm_accounting/EX1_Complete_formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hulaas/Desktop/Projects/midterm_accounting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49165A28-CF84-9E4B-938C-628F0021B290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C27E362-9CA9-104E-8785-BBA317D7B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="14920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="14920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1a" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -539,6 +539,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,7 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -906,6 +912,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2027,8 +2037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F46F1A-FBF1-4BE4-B606-086908F35B7E}">
   <dimension ref="A1:L115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="92" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:C110"/>
+    <sheetView topLeftCell="A81" zoomScale="89" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4189,8 +4199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419DB884-1A68-43C7-806A-1056F0E8519D}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4276,11 +4286,11 @@
         <v>-1499970</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="31" t="s">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="97" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="98">
         <f>C3+C4+C5+C6</f>
         <v>-531063.92000000004</v>
       </c>
@@ -4315,11 +4325,11 @@
         <v>19818.920000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="31" t="s">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="97" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="98">
         <f>C7+C8+C9+C10</f>
         <v>692725</v>
       </c>
@@ -4369,10 +4379,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="99" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="52">
+      <c r="C24" s="100">
         <f>C22+C23</f>
         <v>308322</v>
       </c>

</xml_diff>